<commit_message>
added individual vins for the ss tests: pt2
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Desktop\SUITE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8328"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
     <t>SYMBOL_2000</t>
   </si>
   <si>
-    <t>1GPGP1111&amp;1</t>
+    <t>AAAKN3DD&amp;E</t>
   </si>
 </sst>
 </file>
@@ -559,34 +559,34 @@
   <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="21" max="21" width="22.85546875" customWidth="1"/>
-    <col min="23" max="23" width="22.28515625" customWidth="1"/>
-    <col min="24" max="24" width="20.85546875" customWidth="1"/>
-    <col min="25" max="25" width="34.7109375" customWidth="1"/>
-    <col min="26" max="26" width="5.85546875" customWidth="1"/>
-    <col min="27" max="27" width="16.28515625" customWidth="1"/>
-    <col min="28" max="29" width="13.7109375" customWidth="1"/>
-    <col min="35" max="35" width="19.85546875" customWidth="1"/>
-    <col min="36" max="36" width="21.85546875" customWidth="1"/>
-    <col min="38" max="38" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="24.5546875" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="21" max="21" width="22.88671875" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" customWidth="1"/>
+    <col min="24" max="24" width="20.88671875" customWidth="1"/>
+    <col min="25" max="25" width="34.6640625" customWidth="1"/>
+    <col min="26" max="26" width="5.88671875" customWidth="1"/>
+    <col min="27" max="27" width="16.33203125" customWidth="1"/>
+    <col min="28" max="29" width="13.6640625" customWidth="1"/>
+    <col min="35" max="35" width="19.88671875" customWidth="1"/>
+    <col min="36" max="36" width="21.88671875" customWidth="1"/>
+    <col min="38" max="38" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +702,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -818,7 +818,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -934,7 +934,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
added individual vins for the ss tests: pt3 SS
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
@@ -212,7 +212,7 @@
     <t>SYMBOL_2000</t>
   </si>
   <si>
-    <t>AAAKN3DD&amp;E</t>
+    <t>BBBKN3DD&amp;E</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed pas11659 Renewal Version 35 and 45 tests, updated VIN tables to get tests working
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reps\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -546,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added xls data for  TestVINUpload.pas11659_Renewal_VersionR45 CacheManager click changed to javascript click
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reps\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="78">
   <si>
     <t>VIN</t>
   </si>
@@ -140,9 +140,6 @@
     <t>B-IMMOBILIZER/KEYLSS ENTRY/ALARM</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -182,25 +179,85 @@
     <t>Gt</t>
   </si>
   <si>
+    <t>invalidVIN</t>
+  </si>
+  <si>
+    <t>SecondValid</t>
+  </si>
+  <si>
+    <t>ThirdValid</t>
+  </si>
+  <si>
+    <t>TOYOTA</t>
+  </si>
+  <si>
+    <t>SYMBOL_2000</t>
+  </si>
+  <si>
+    <t>BBBKN3DD&amp;E</t>
+  </si>
+  <si>
+    <t>BI001</t>
+  </si>
+  <si>
+    <t>PD001</t>
+  </si>
+  <si>
+    <t>UM001</t>
+  </si>
+  <si>
+    <t>MP001</t>
+  </si>
+  <si>
+    <t>BI002</t>
+  </si>
+  <si>
+    <t>BI003</t>
+  </si>
+  <si>
+    <t>BI004</t>
+  </si>
+  <si>
+    <t>PD002</t>
+  </si>
+  <si>
+    <t>PD003</t>
+  </si>
+  <si>
+    <t>PD004</t>
+  </si>
+  <si>
+    <t>UM002</t>
+  </si>
+  <si>
+    <t>UM003</t>
+  </si>
+  <si>
+    <t>UM004</t>
+  </si>
+  <si>
+    <t>MP002</t>
+  </si>
+  <si>
+    <t>MP003</t>
+  </si>
+  <si>
+    <t>MP004</t>
+  </si>
+  <si>
+    <t>SYMBOL_2017</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
-    <t>invalidVIN</t>
-  </si>
-  <si>
-    <t>SecondValid</t>
-  </si>
-  <si>
-    <t>ThirdValid</t>
-  </si>
-  <si>
-    <t>TOYOTA</t>
-  </si>
-  <si>
-    <t>SYMBOL_2000</t>
-  </si>
-  <si>
-    <t>BBBKN3DD&amp;E</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -544,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,48 +717,48 @@
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>28</v>
@@ -713,19 +770,19 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="3">
         <v>8</v>
@@ -767,51 +824,51 @@
         <v>42</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="AG2" s="3">
         <v>20010101</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -823,19 +880,19 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" s="3">
         <v>8</v>
@@ -877,51 +934,51 @@
         <v>42</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="AG3" s="3">
         <v>20000101</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>28</v>
@@ -933,19 +990,19 @@
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4" s="3">
         <v>8</v>
@@ -987,51 +1044,51 @@
         <v>42</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="AG4" s="3">
         <v>20150101</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>28</v>
@@ -1043,19 +1100,19 @@
         <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O5" s="3">
         <v>8</v>
@@ -1097,31 +1154,471 @@
         <v>42</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="AG5" s="3">
         <v>20190101</v>
       </c>
       <c r="AH5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3">
+        <v>53080</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI5" s="3" t="s">
+      <c r="O6" s="3">
+        <v>8</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>214</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" s="3">
+        <v>2</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="3">
+        <v>2</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>42</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>20010101</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3">
+        <v>53080</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AJ5" s="3" t="s">
-        <v>49</v>
+      <c r="O7" s="3">
+        <v>8</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>214</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="3">
+        <v>2</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="3">
+        <v>2</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>42</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>20000101</v>
+      </c>
+      <c r="AH7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3">
+        <v>53080</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="3">
+        <v>8</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>214</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" s="3">
+        <v>2</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="3">
+        <v>2</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>42</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>42</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>20150101</v>
+      </c>
+      <c r="AH8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="3">
+        <v>53080</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="3">
+        <v>8</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>214</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9" s="3">
+        <v>2</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="3">
+        <v>2</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>42</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>42</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>20190101</v>
+      </c>
+      <c r="AH9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ9" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>